<commit_message>
Asignar y ver aulas asignadas
</commit_message>
<xml_diff>
--- a/SCRUM/Historias de usuario.xlsx
+++ b/SCRUM/Historias de usuario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jreye\Documents\TecNMCampusCuliacan\Git Repositories\Sistema-Incidencias\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506A7C28-DCEB-442A-B53E-D16DF61DF95C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D92485-1C9C-43A3-8F82-9A851615D6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C0C8A035-E5AC-4480-B3F8-78550C33012A}"/>
   </bookViews>
@@ -335,59 +335,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -705,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987422C4-3F7F-4AB0-B20B-C90837CC6BBE}">
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,478 +717,478 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="16"/>
+      <c r="I2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19">
+      <c r="H3" s="14"/>
+      <c r="I3" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="19">
+      <c r="H4" s="14"/>
+      <c r="I4" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="14" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="2">
+      <c r="H5" s="14"/>
+      <c r="I5" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="9"/>
+      <c r="H6" s="10"/>
       <c r="I6" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="9" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9" t="s">
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="9"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="14" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="9" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="10"/>
       <c r="I8" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="14" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="9" t="s">
+      <c r="D9" s="12"/>
+      <c r="E9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="9"/>
+      <c r="H9" s="10"/>
       <c r="I9" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="11" t="s">
+      <c r="D10" s="19"/>
+      <c r="E10" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11" t="s">
+      <c r="F10" s="20"/>
+      <c r="G10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="4">
+      <c r="H10" s="20"/>
+      <c r="I10" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="9" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="9"/>
+      <c r="H11" s="10"/>
       <c r="I11" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="9" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="9"/>
+      <c r="H12" s="10"/>
       <c r="I12" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8" t="s">
+      <c r="D13" s="13"/>
+      <c r="E13" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8" t="s">
+      <c r="F13" s="17"/>
+      <c r="G13" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="8"/>
+      <c r="H13" s="17"/>
       <c r="I13" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="8" t="s">
+      <c r="D14" s="13"/>
+      <c r="E14" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8" t="s">
+      <c r="F14" s="17"/>
+      <c r="G14" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="6">
+      <c r="H14" s="17"/>
+      <c r="I14" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="9" t="s">
+      <c r="D15" s="13"/>
+      <c r="E15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="6">
+      <c r="H15" s="10"/>
+      <c r="I15" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8" t="s">
+      <c r="F16" s="9"/>
+      <c r="G16" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="6">
+      <c r="H16" s="9"/>
+      <c r="I16" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8" t="s">
+      <c r="D17" s="8"/>
+      <c r="E17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8" t="s">
+      <c r="F17" s="9"/>
+      <c r="G17" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="6">
+      <c r="H17" s="9"/>
+      <c r="I17" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7" t="s">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8" t="s">
+      <c r="D18" s="8"/>
+      <c r="E18" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8" t="s">
+      <c r="F18" s="9"/>
+      <c r="G18" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="6">
+      <c r="H18" s="9"/>
+      <c r="I18" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7" t="s">
+      <c r="B19" s="13"/>
+      <c r="C19" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8" t="s">
+      <c r="D19" s="13"/>
+      <c r="E19" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8" t="s">
+      <c r="F19" s="17"/>
+      <c r="G19" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="6">
+      <c r="H19" s="17"/>
+      <c r="I19" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8" t="s">
+      <c r="D20" s="8"/>
+      <c r="E20" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8" t="s">
+      <c r="F20" s="9"/>
+      <c r="G20" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="6">
+      <c r="H20" s="9"/>
+      <c r="I20" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="20" t="s">
+      <c r="D21" s="8"/>
+      <c r="E21" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20" t="s">
+      <c r="F21" s="9"/>
+      <c r="G21" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H21" s="20"/>
-      <c r="I21" s="21">
+      <c r="H21" s="9"/>
+      <c r="I21" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16" t="s">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="20" t="s">
+      <c r="D22" s="8"/>
+      <c r="E22" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20" t="s">
+      <c r="F22" s="9"/>
+      <c r="G22" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H22" s="20"/>
-      <c r="I22" s="21">
+      <c r="H22" s="9"/>
+      <c r="I22" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="20" t="s">
+      <c r="D23" s="8"/>
+      <c r="E23" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20" t="s">
+      <c r="F23" s="9"/>
+      <c r="G23" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H23" s="20"/>
-      <c r="I23" s="21">
+      <c r="H23" s="9"/>
+      <c r="I23" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1200,39 +1200,61 @@
     <row r="29" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1048576" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E1048576" s="9" t="s">
+      <c r="E1048576" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F1048576" s="9"/>
+      <c r="F1048576" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="E1048576:F1048576"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E3:F3"/>
@@ -1249,54 +1271,32 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="E1048576:F1048576"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>